<commit_message>
load (badly) done, execute kinda done
</commit_message>
<xml_diff>
--- a/points/points.xlsx
+++ b/points/points.xlsx
@@ -477,7 +477,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,7 @@
         <v>0.4</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E12" si="1">B3*0.3</f>
+        <f t="shared" ref="E3:E6" si="1">B3*0.3</f>
         <v>2.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
unalmas az opreh előadás
</commit_message>
<xml_diff>
--- a/points/points.xlsx
+++ b/points/points.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Beadás</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>MAX:</t>
+  </si>
+  <si>
+    <t>Minden részből a pontok 41%-a kell min</t>
   </si>
 </sst>
 </file>
@@ -493,12 +496,12 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -572,7 +575,7 @@
         <v>0.96666666666666667</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E3:E6" si="1">B4*0.3</f>
+        <f t="shared" ref="E4:E6" si="1">B4*0.3</f>
         <v>8.6999999999999993</v>
       </c>
     </row>
@@ -776,6 +779,11 @@
       <c r="E13" s="10">
         <f xml:space="preserve"> SUM(E2:E12)</f>
         <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.25">

</xml_diff>